<commit_message>
GFG array rearrangement #1
</commit_message>
<xml_diff>
--- a/session4/Progress.xlsx
+++ b/session4/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C284E6A7-DE57-42AA-9AAA-46A2258D7C30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA06CE9-5EE5-4B8D-9FD4-965966D3835E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Leetcode</t>
   </si>
@@ -58,13 +58,62 @@
   </si>
   <si>
     <t>Array Rotation 6</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/given-a-sorted-and-rotated-array-find-if-there-is-a-pair-with-a-given-sum/</t>
+  </si>
+  <si>
+    <t>Array Rotation 7</t>
+  </si>
+  <si>
+    <t>no idea</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/find-maximum-value-of-sum-iarri-with-only-rotations-on-given-array-allowed/</t>
+  </si>
+  <si>
+    <t>no idea
+based on prev #7</t>
+  </si>
+  <si>
+    <t>Array Rotation 8</t>
+  </si>
+  <si>
+    <t>Array Rotation 9</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/find-rotation-count-rotated-sorted-array/</t>
+  </si>
+  <si>
+    <t>based on q#5 finding pivot</t>
+  </si>
+  <si>
+    <t>Array Rotation 10</t>
+  </si>
+  <si>
+    <t>similar</t>
+  </si>
+  <si>
+    <t>Array Rotation 11</t>
+  </si>
+  <si>
+    <t>Array Rotation 12</t>
+  </si>
+  <si>
+    <t>finding pivot which is min</t>
+  </si>
+  <si>
+    <t>Array Rotation 13</t>
+  </si>
+  <si>
+    <t>useless brute force</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +125,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,10 +157,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -387,15 +445,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.26953125" customWidth="1"/>
+    <col min="3" max="3" width="19.90625" customWidth="1"/>
     <col min="4" max="5" width="8.7265625" customWidth="1"/>
     <col min="6" max="6" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -443,13 +502,88 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2">
+        <v>43979</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" xr:uid="{3AF05B12-E336-4706-B10A-609E755AFA2E}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{1AEC65F1-55C3-46E5-9C8C-AB53C6F13C21}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{F9F0B929-A21F-49DC-BD5B-D06C2FBA0A84}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{A14CDD69-9C89-472B-9609-652DDF8A87FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
GFG Array Rearrangement 2
</commit_message>
<xml_diff>
--- a/session4/Progress.xlsx
+++ b/session4/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA06CE9-5EE5-4B8D-9FD4-965966D3835E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D03CA87-B75A-4E99-A049-C2827CEF141C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Leetcode</t>
   </si>
@@ -107,13 +107,28 @@
   </si>
   <si>
     <t>useless brute force</t>
+  </si>
+  <si>
+    <t>Array Rearrangement 1</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/rearrange-array-arri/</t>
+  </si>
+  <si>
+    <t>Array Rearrangement 2</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/write-a-program-to-reverse-an-array-or-string/</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +140,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,12 +180,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -445,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -456,24 +485,28 @@
     <col min="1" max="1" width="10.26953125" customWidth="1"/>
     <col min="3" max="3" width="19.90625" customWidth="1"/>
     <col min="4" max="5" width="8.7265625" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>2</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -577,14 +610,41 @@
         <v>25</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2">
+        <v>43980</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" xr:uid="{3AF05B12-E336-4706-B10A-609E755AFA2E}"/>
     <hyperlink ref="G4" r:id="rId2" xr:uid="{1AEC65F1-55C3-46E5-9C8C-AB53C6F13C21}"/>
     <hyperlink ref="G5" r:id="rId3" xr:uid="{F9F0B929-A21F-49DC-BD5B-D06C2FBA0A84}"/>
     <hyperlink ref="G7" r:id="rId4" xr:uid="{A14CDD69-9C89-472B-9609-652DDF8A87FF}"/>
+    <hyperlink ref="G13" r:id="rId5" xr:uid="{3126909B-7EAC-4538-A996-3DF9BEB8CE87}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
gfg array rearrange 3
</commit_message>
<xml_diff>
--- a/session4/Progress.xlsx
+++ b/session4/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D03CA87-B75A-4E99-A049-C2827CEF141C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DC31A7-62B6-4E6C-874E-3162B79DB5AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,19 +109,19 @@
     <t>useless brute force</t>
   </si>
   <si>
-    <t>Array Rearrangement 1</t>
-  </si>
-  <si>
     <t>https://www.geeksforgeeks.org/rearrange-array-arri/</t>
   </si>
   <si>
-    <t>Array Rearrangement 2</t>
-  </si>
-  <si>
     <t>https://www.geeksforgeeks.org/write-a-program-to-reverse-an-array-or-string/</t>
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>Array Rearrangement #1</t>
+  </si>
+  <si>
+    <t>Array Rearrangement #2</t>
   </si>
 </sst>
 </file>
@@ -476,16 +476,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.26953125" customWidth="1"/>
     <col min="3" max="3" width="19.90625" customWidth="1"/>
-    <col min="4" max="5" width="8.7265625" customWidth="1"/>
-    <col min="6" max="6" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="4.90625" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -506,7 +508,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -618,10 +620,10 @@
         <v>43980</v>
       </c>
       <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" t="s">
         <v>27</v>
-      </c>
-      <c r="G12" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -629,10 +631,10 @@
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GFG array rearrangement q4
</commit_message>
<xml_diff>
--- a/session4/Progress.xlsx
+++ b/session4/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DC31A7-62B6-4E6C-874E-3162B79DB5AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DE8214-C56E-45FA-93CD-9B25E2BBCC22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Leetcode</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>Array Rearrangement #2</t>
+  </si>
+  <si>
+    <t>Array Rearrangement #3</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/rearrange-array-arri-arrj-even-arri/</t>
+  </si>
+  <si>
+    <t>Array Rearrangement #4</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/rearrange-positive-and-negative-numbers-publish/</t>
   </si>
 </sst>
 </file>
@@ -474,11 +486,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -637,6 +649,28 @@
         <v>28</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -645,8 +679,9 @@
     <hyperlink ref="G5" r:id="rId3" xr:uid="{F9F0B929-A21F-49DC-BD5B-D06C2FBA0A84}"/>
     <hyperlink ref="G7" r:id="rId4" xr:uid="{A14CDD69-9C89-472B-9609-652DDF8A87FF}"/>
     <hyperlink ref="G13" r:id="rId5" xr:uid="{3126909B-7EAC-4538-A996-3DF9BEB8CE87}"/>
+    <hyperlink ref="G15" r:id="rId6" xr:uid="{A62102DA-0AE3-4059-9B77-E53BEA33D072}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
leetcode 378 GFG array q6
</commit_message>
<xml_diff>
--- a/session4/Progress.xlsx
+++ b/session4/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HB\Masters\College_Docs\SJSU\MS-SE_courses\GitHub_stuff\Data-Structures-Algorithms_practice\session4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9684645C-AFA9-42AB-8AD7-4FF685A3F318}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E20F0A-713A-4FF8-B709-58A679B3C238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>Leetcode</t>
   </si>
@@ -167,6 +167,18 @@
   </si>
   <si>
     <t>https://www.geeksforgeeks.org/minimum-swaps-required-bring-elements-less-equal-k-together/</t>
+  </si>
+  <si>
+    <t>Array Order Statistics #1</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/kth-smallestlargest-element-unsorted-array/</t>
+  </si>
+  <si>
+    <t>Array Order Statistics #6</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/kth-smallest-element-in-a-row-wise-and-column-wise-sorted-2d-array-set-1/</t>
   </si>
 </sst>
 </file>
@@ -519,11 +531,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -715,7 +727,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>39</v>
       </c>
@@ -726,7 +738,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>42</v>
       </c>
@@ -734,7 +746,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
         <v>44</v>
       </c>
@@ -746,6 +758,40 @@
       </c>
       <c r="G19" s="1" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>215</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>378</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -759,8 +805,9 @@
     <hyperlink ref="G15" r:id="rId6" xr:uid="{A62102DA-0AE3-4059-9B77-E53BEA33D072}"/>
     <hyperlink ref="G17" r:id="rId7" xr:uid="{0A3AD2EB-DF36-403E-B624-0BD2D2FD7103}"/>
     <hyperlink ref="G19" r:id="rId8" xr:uid="{3549B9FF-7C5A-4AD5-9AF9-C18E344A769A}"/>
+    <hyperlink ref="G21" r:id="rId9" xr:uid="{6C5F3009-BA62-4FFF-8069-7F551E4EBA49}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>